<commit_message>
EPBDS: added hints support.
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/DefaultCustomConvertersTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/DefaultCustomConvertersTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="24735" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C8:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -850,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="D5:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,7 +925,7 @@
   <dimension ref="C5:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>